<commit_message>
updated proportion of distractors so that n distractor = n targets
</commit_message>
<xml_diff>
--- a/scene_cat_exp_2023.2.2/input_files/10_scenecat_block_order.xlsx
+++ b/scene_cat_exp_2023.2.2/input_files/10_scenecat_block_order.xlsx
@@ -360,22 +360,22 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>living_rooms_1</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
           <t>bedrooms_1</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>kitchens_1</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>living_rooms_1</t>
+        </is>
+      </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>bedrooms_2</t>
+          <t>kitchens_2</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -385,16 +385,16 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>kitchens_2</t>
+          <t>bedrooms_2</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -417,10 +417,10 @@
         <v>0</v>
       </c>
       <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
         <v>1</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -431,19 +431,19 @@
     </row>
     <row r="4">
       <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
         <v>1</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -460,13 +460,13 @@
         <v>0</v>
       </c>
       <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
         <v>1</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -474,7 +474,7 @@
         <v>0</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -486,7 +486,7 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -497,13 +497,13 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>0</v>

</xml_diff>

<commit_message>
Cleaned up the image folder. Removed text labels from some .png files.
</commit_message>
<xml_diff>
--- a/scene_cat_exp_2023.2.2/input_files/10_scenecat_block_order.xlsx
+++ b/scene_cat_exp_2023.2.2/input_files/10_scenecat_block_order.xlsx
@@ -360,12 +360,12 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>bedrooms_1</t>
+          <t>kitchens_1</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>kitchens_1</t>
+          <t>bedrooms_1</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -375,12 +375,12 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>kitchens_2</t>
+          <t>living_rooms_2</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>living_rooms_2</t>
+          <t>kitchens_2</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -391,10 +391,10 @@
     </row>
     <row r="2">
       <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
         <v>1</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -420,10 +420,10 @@
         <v>0</v>
       </c>
       <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
         <v>1</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -440,10 +440,10 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -471,10 +471,10 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <v>0</v>

</xml_diff>